<commit_message>
add the missed stringr package
</commit_message>
<xml_diff>
--- a/lnHako.xlsx
+++ b/lnHako.xlsx
@@ -25,18 +25,18 @@
     <t>description</t>
   </si>
   <si>
+    <t>artists</t>
+  </si>
+  <si>
+    <t>authors</t>
+  </si>
+  <si>
     <t>publishers</t>
   </si>
   <si>
     <t>imgName</t>
   </si>
   <si>
-    <t>artists</t>
-  </si>
-  <si>
-    <t>authors</t>
-  </si>
-  <si>
     <t>publisherID</t>
   </si>
   <si>
@@ -163,24 +163,6 @@
     <t>BOOK20</t>
   </si>
   <si>
-    <t>Holmes ở Kyoto - Tập 3</t>
-  </si>
-  <si>
-    <t>Bạn Gái Vs. Bạn Thời Thơ Ấu - Tập 5</t>
-  </si>
-  <si>
-    <t>OVERLORD - Tập 4: Lizardman Anh Dũng</t>
-  </si>
-  <si>
-    <t>Date A Live - Tập 11</t>
-  </si>
-  <si>
-    <t>Gate: Lực Lượng Phòng Vệ Chiến Đấu Ở Tân Thế Giới - Tập 1</t>
-  </si>
-  <si>
-    <t>Những Lời Chúng Tôi Nói Ở Bệnh Viện Bên Bờ Biển</t>
-  </si>
-  <si>
     <t>86 Eighty Six - Ep.2</t>
   </si>
   <si>
@@ -223,23 +205,22 @@
     <t>Em Là Ánh Sáng Giữa Đêm Trăng</t>
   </si>
   <si>
-    <t>Trong tập 3 này, Kyoto đã bước vào tháng Mười Một, khi sự hiện diện của mùa đông đã bắt đầu trở nên rõ nét. Hôm nay, Mashiro Aoi vẫn cùng chàng trai kinh kì "nham hiểm" Yagashira Kiyotaka làm việc tại cửa hàng đồ cổ "Kura" ở phố mua sắm Teramachi Sanjo.Một ngày nọ, diễn viên Kabuki nổi tiếng Ichikat...</t>
-  </si>
-  <si>
-    <t>Kỳ tập huấn hè kết thúc bằng lời tỏ tình bất ngờ từ Chiwa. Câu chuyện về những cô gái nhe nanh múa vuốt hướng đến học kỳ hai trong tiếng trống trận chiến trường khốc liệt vang lên. Trong tập này ghi lại câu chuyện Eita cùng với Chiwa đi về trường cấp hai cũ! Đối đầu với ủy ban kỷ luật vì chuyện liên...</t>
-  </si>
-  <si>
-    <t>Overlord kể về Suzuki Satoru, hay Ainz, một nhân viên văn phòng say mê tâm huyết với game ruột YGGDRASIL đến mức đồng đội gắn bó một thời đã lần lượt rời xa, chính cái game cũng sắp dừng hoạt động, anh vẫn đăng nhập để nhâm nhi hoài niệm và đi cùng nó những phút giây sau cuối.
-Giờ kết thúc đã điểm,...</t>
-  </si>
-  <si>
-    <t>Cô gái đã trở thành Tinh linh thứ 8 – Tobiichi Origami.Cô gái căm thù Tinh linh ấy đã sở hữu sức mạnh mà mình mong muốn. Để tìm ra kẻ sát nhân giết hại bố mẹ mình, cô ấy đã mượn sức mạnh của Kurumi và trở lại thành phố Tenguu năm năm về trước. Nhưng tại đây, những điều hiển hiện trước mắt cô ấy thật...</t>
-  </si>
-  <si>
-    <t>Năm 20xx.Giữa một trưa nắng nóng tại khu G, thành phố T, một Cánh cổng dẫn đến thế giới khác đột nhiên xuất hiện.Từ trong Cánh cổng tràn ra một đội quân quái vật từ thế giới bên kia, ra tay thảm sát biến khu vực G thành địa ngục trong nháy mắt. Bằng vũ khí và chiến thuật áp đảo, Lực lượng phòng vệ n...</t>
-  </si>
-  <si>
-    <t>Một năm trước đã xảy ra một "cuộc chiến". Căn bệnh kì lạ nọ đột nhiên phát tán ở một địa phương hẻo lánh và lan rộng. Hàng ngàn người đã thiệt mạng, phần đông trong số đó là người lớn. Nhưng có vẻ như một số thiếu niên sống sót lại phát triển những sức mạnh siêu việt từ căn bệnh. Và cùng với căn bện...</t>
+    <t>Sakurako Và Bộ Xương Dưới Gốc Anh Đào - Tập 7</t>
+  </si>
+  <si>
+    <t>Biên Niên Sử Đế Chế Alexis - Tập 8</t>
+  </si>
+  <si>
+    <t>Date A Live Encore 2</t>
+  </si>
+  <si>
+    <t>Hướng Dẫn Sử Dụng Thiên Sứ Vụng Về</t>
+  </si>
+  <si>
+    <t>Liệu Có Sai Lầm Khi Tìm Kiếm Cuộc Gặp Gỡ Định Mệnh Trong Dungeon? - Tập 4</t>
+  </si>
+  <si>
+    <t>Anohana - Đóa Hoa Ngày Ấy</t>
   </si>
   <si>
     <t>Sau khi từ biệt Lena, nữ Handler của Cộng hòa, nhóm Tám Sáu do Shin dẫn đầu được nước láng giềng Liên bang Giad đón nhận. Tại đây, họ được trao cơ hội hưởng hòa bình và tự do. Nhưng chỉ sau một thời gian nghỉ ngơi ngắn, họ đã chọn quay lại chiến trường.
@@ -290,46 +271,160 @@
 Bọn họ vốn học cùng lớp nhưng chưa từng gặp nhau, không biết tên nhau. Là do cô mắc bệnh nan y, không thể tách xa môi trường thuốc men và cấp cứu của bệnh viện. Là...</t>
   </si>
   <si>
+    <t>Hokkaido, mùa đông Asahikawa. Tôi – Shoutarou – được cô Shouko vốn thân thiết với Sakurako mời đến biệt thự ở Asahidake để dọn dẹp di vật của người chủ. Thật ngạc nhiên, Sakurako vốn chẳng hứng thú với điều gì ngoài xương và bí ẩn cũng cùng đi.
+Sau khi đã chơi đùa thoả thuê trên núi tuyết, chúng tôi...</t>
+  </si>
+  <si>
+    <t>Đế quốc Amadof thất thủ! Leonart trở thành người đứng đầu cả một vương quốc. Tin tức này làm chấn động các nước lân cận, ngay cả "Hoàng Tử Máu Lạnh" Circus – người đang trên đường hành quân đến Palidida – cũng nắm rõ.
+"Chính là lúc này. Đến giành lấy lãnh địa của ta nào."
+Mặt khác, tin tức về sự trỗ...</t>
+  </si>
+  <si>
+    <t>“Giờ thì, hôn... hôn mình đi nào!”Vào một ngày nọ, không hiểu sao mà cả hội ‘Tinh Linh’ đều ráo riết truy đòi một nụ hôn từ Itsuka Shidou.“Ai đánh thức được bản năng đàn ông trong người anh ta sẽ là người chiến thắng!”
+Trong kỳ nghỉ hè tại một lữ quán suối nước nóng, hội ‘Tinh Linh’ đã bí mật tổ chứ...</t>
+  </si>
+  <si>
+    <t>Cuối tháng Ba, một ngày trước lễ khai giảng cấp ba, Minemoto Shinya - một cựu otaku đã quyết định thoát khỏi địa ngục mang tên “sáng tác” nhằm tận hưởng cuộc sống học đường như một người bình thường. Tuy nhiên, quyết tâm ấy chẳng bao lâu đã vấp phải trở ngại: Cô bạn cùng lớp Mezaki Rin đã phát hiện...</t>
+  </si>
+  <si>
+    <t>“CẤP ĐỘ HAI!!??”
+Sau khi đánh bại Minotaur ở tập trước, Bell trở thành người nắm giữ kỉ lục thăng cấp nhanh nhất thế giới (hay còn được gọi là Cậu Thỏ Nhanh Nhất Thế Giới). Tuy bỗng chốc đã thu hút được biết bao sự chú ý và ghen tị ở Orario, cậu lại không thể tìm được người để mời làm đồng đội. Giữa...</t>
+  </si>
+  <si>
+    <t>Mãi mãi là bạn tốt…
+Thời thơ ấu, nhóm bạn thân sáu người với danh xưng “Super Peace Busters” luôn như hình với bóng. Tuy nhiên khi lên cấp ba, họ lại trở nên xa cách. Jintan tự giam mình trong nhà. Anaru gắng gượng hòa nhập với hội bạn gái thời thượng. Yukiatsu và Tsuruko cùng học trường điểm có tiế...</t>
+  </si>
+  <si>
+    <t>Shirabii</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Take</t>
+  </si>
+  <si>
+    <t>Shinotsuki Shinobu</t>
+  </si>
+  <si>
+    <t>Ayakura Juu</t>
+  </si>
+  <si>
+    <t>Mizoguchi Keeji</t>
+  </si>
+  <si>
+    <t>Fal Maro</t>
+  </si>
+  <si>
+    <t>Takaya-Ki</t>
+  </si>
+  <si>
+    <t>Shirai Eiri</t>
+  </si>
+  <si>
+    <t>Zaza</t>
+  </si>
+  <si>
+    <t>Haga Yui</t>
+  </si>
+  <si>
+    <t>Truffle, Kei</t>
+  </si>
+  <si>
+    <t>Tetsuo</t>
+  </si>
+  <si>
+    <t>Tamago no Kimi</t>
+  </si>
+  <si>
+    <t>Tsunako</t>
+  </si>
+  <si>
+    <t>Machimura Komori</t>
+  </si>
+  <si>
+    <t>Yasuda Suzuhito</t>
+  </si>
+  <si>
+    <t>Asato Asato</t>
+  </si>
+  <si>
+    <t>Sakuraba Kazuki</t>
+  </si>
+  <si>
+    <t>Nisioisin</t>
+  </si>
+  <si>
+    <t>Carlo Zen</t>
+  </si>
+  <si>
+    <t>Hasekura Isuna</t>
+  </si>
+  <si>
+    <t>Kamoshida Hajime</t>
+  </si>
+  <si>
+    <t>Toba Toru</t>
+  </si>
+  <si>
+    <t>Shirakome Ryou</t>
+  </si>
+  <si>
+    <t>Jyumonji Ao</t>
+  </si>
+  <si>
+    <t>SOW</t>
+  </si>
+  <si>
+    <t>Inoue Kenji</t>
+  </si>
+  <si>
+    <t>CHIROLU</t>
+  </si>
+  <si>
+    <t>Sano Tetsuya</t>
+  </si>
+  <si>
+    <t>Oota Shiori</t>
+  </si>
+  <si>
+    <t>Awamura Akamitsu</t>
+  </si>
+  <si>
+    <t>Tachibana Koushi</t>
+  </si>
+  <si>
+    <t>Kuroki Satoki</t>
+  </si>
+  <si>
+    <t>Omori Fujino</t>
+  </si>
+  <si>
+    <t>Okada Mari</t>
+  </si>
+  <si>
+    <t>IPM</t>
+  </si>
+  <si>
     <t>Kim Đồng</t>
   </si>
   <si>
-    <t>Uranix</t>
-  </si>
-  <si>
-    <t>IPM</t>
+    <t>Nhã Nam</t>
+  </si>
+  <si>
+    <t>Thái Hà Books</t>
+  </si>
+  <si>
+    <t>Tsuki Light Novel</t>
   </si>
   <si>
     <t>Amak</t>
   </si>
   <si>
-    <t>Nhã Nam</t>
-  </si>
-  <si>
-    <t>Thái Hà Books</t>
-  </si>
-  <si>
-    <t>Tsuki Light Novel</t>
-  </si>
-  <si>
     <t>Sky Light Novel</t>
   </si>
   <si>
-    <t>CuoiKy\HakoImg\u2-32adabcc-18e1-4b12-be80-c5b96cfeb25b.jpg</t>
-  </si>
-  <si>
-    <t>CuoiKy\HakoImg\u2-f38fc32e-d672-4a5c-940b-d3d39e22e9ce.jpg</t>
-  </si>
-  <si>
-    <t>CuoiKy\HakoImg\u2-0aac9576-7c2c-4a08-a87f-e278532f5230.jpg</t>
-  </si>
-  <si>
-    <t>CuoiKy\HakoImg\u2-5adce8cb-6e6b-4a29-91f5-147c3478c17f.jpg</t>
-  </si>
-  <si>
-    <t>CuoiKy\HakoImg\u2-9574e27a-8fbf-4bd7-9c69-036cc5a8971f.jpg</t>
-  </si>
-  <si>
-    <t>CuoiKy\HakoImg\u2-9b794ab1-dd7e-4619-9dda-1f3a42bbbccb.jpg</t>
+    <t>Shine Novel</t>
   </si>
   <si>
     <t>CuoiKy\HakoImg\u2-e964fe9f-c4e8-4f6d-a6bf-fa1f9a77efb3.jpg</t>
@@ -374,112 +469,22 @@
     <t>CuoiKy\HakoImg\u2-6b83ee96-318f-4f7c-9795-43c1709955ac.jpg</t>
   </si>
   <si>
-    <t>Yamouchishizu</t>
-  </si>
-  <si>
-    <t>Ruroo</t>
-  </si>
-  <si>
-    <t>So-bin</t>
-  </si>
-  <si>
-    <t>Tsunako</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Yoneyama Mai</t>
-  </si>
-  <si>
-    <t>Shirabii</t>
-  </si>
-  <si>
-    <t>Take</t>
-  </si>
-  <si>
-    <t>Shinotsuki Shinobu</t>
-  </si>
-  <si>
-    <t>Ayakura Juu</t>
-  </si>
-  <si>
-    <t>Mizoguchi Keeji</t>
-  </si>
-  <si>
-    <t>Fal Maro</t>
-  </si>
-  <si>
-    <t>Takaya-Ki</t>
-  </si>
-  <si>
-    <t>Shirai Eiri</t>
-  </si>
-  <si>
-    <t>Zaza</t>
-  </si>
-  <si>
-    <t>Haga Yui</t>
-  </si>
-  <si>
-    <t>Truffle, Kei</t>
-  </si>
-  <si>
-    <t>Mochizuki Mai</t>
-  </si>
-  <si>
-    <t>Yuuji Yuuji</t>
-  </si>
-  <si>
-    <t>Maruyama Kugane</t>
-  </si>
-  <si>
-    <t>Tachibana Koushi</t>
-  </si>
-  <si>
-    <t>Yanai Takumi</t>
-  </si>
-  <si>
-    <t>Ishikawa Hiroshi</t>
-  </si>
-  <si>
-    <t>Asato Asato</t>
-  </si>
-  <si>
-    <t>Sakuraba Kazuki</t>
-  </si>
-  <si>
-    <t>Nisioisin</t>
-  </si>
-  <si>
-    <t>Carlo Zen</t>
-  </si>
-  <si>
-    <t>Hasekura Isuna</t>
-  </si>
-  <si>
-    <t>Kamoshida Hajime</t>
-  </si>
-  <si>
-    <t>Toba Toru</t>
-  </si>
-  <si>
-    <t>Shirakome Ryou</t>
-  </si>
-  <si>
-    <t>Jyumonji Ao</t>
-  </si>
-  <si>
-    <t>SOW</t>
-  </si>
-  <si>
-    <t>Inoue Kenji</t>
-  </si>
-  <si>
-    <t>CHIROLU</t>
-  </si>
-  <si>
-    <t>Sano Tetsuya</t>
+    <t>CuoiKy\HakoImg\u2-9ea5354f-95d5-45d7-aa18-00b884c07432.jpg</t>
+  </si>
+  <si>
+    <t>CuoiKy\HakoImg\u2-2454ce0b-9af1-46b6-9328-def2bbb30af5.jpg</t>
+  </si>
+  <si>
+    <t>CuoiKy\HakoImg\u2-cf76be36-fb8f-45dd-b739-21ebab90e5df.jpg</t>
+  </si>
+  <si>
+    <t>CuoiKy\HakoImg\u2-a747aa3a-52be-4391-9641-e9fa303bea13.jpg</t>
+  </si>
+  <si>
+    <t>CuoiKy\HakoImg\u2-24ccf54e-f598-4ea6-b9b9-79df70d3cef3.jpg</t>
+  </si>
+  <si>
+    <t>CuoiKy\HakoImg\u2-2204e403-02b1-4f63-8d97-98c9325eff6a.jpg</t>
   </si>
   <si>
     <t>PUB1</t>
@@ -652,13 +657,13 @@
         <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="G2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="H2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I2" t="s">
         <v>152</v>
@@ -684,13 +689,13 @@
         <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="G3" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I3" t="s">
         <v>153</v>
@@ -716,13 +721,13 @@
         <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="G4" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="H4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I4" t="s">
         <v>154</v>
@@ -748,13 +753,13 @@
         <v>91</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="G5" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="H5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I5" t="s">
         <v>155</v>
@@ -777,16 +782,16 @@
         <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="G6" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="H6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I6" t="s">
         <v>155</v>
@@ -809,19 +814,19 @@
         <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="G7" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J7" t="s">
         <v>165</v>
@@ -841,19 +846,19 @@
         <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F8" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="G8" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="H8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J8" t="s">
         <v>166</v>
@@ -873,22 +878,22 @@
         <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F9" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="G9" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="H9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I9" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="J9" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10">
@@ -905,22 +910,22 @@
         <v>77</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F10" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="G10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11">
@@ -937,22 +942,22 @@
         <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F11" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G11" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="H11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12">
@@ -969,22 +974,22 @@
         <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F12" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="G12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I12" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13">
@@ -1001,22 +1006,22 @@
         <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="F13" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="G13" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I13" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="J13" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14">
@@ -1030,19 +1035,19 @@
         <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F14" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="G14" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I14" t="s">
         <v>158</v>
@@ -1062,25 +1067,25 @@
         <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="G15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J15" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16">
@@ -1094,25 +1099,25 @@
         <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="G16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I16" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="J16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17">
@@ -1126,25 +1131,25 @@
         <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F17" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="G17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18">
@@ -1158,25 +1163,25 @@
         <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="G18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I18" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19">
@@ -1190,25 +1195,25 @@
         <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="G19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I19" t="s">
         <v>159</v>
       </c>
       <c r="J19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20">
@@ -1225,19 +1230,19 @@
         <v>86</v>
       </c>
       <c r="E20" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="F20" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="G20" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="H20" t="s">
         <v>150</v>
       </c>
       <c r="I20" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="J20" t="s">
         <v>176</v>
@@ -1257,22 +1262,22 @@
         <v>87</v>
       </c>
       <c r="E21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F21" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="G21" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="H21" t="s">
         <v>151</v>
       </c>
       <c r="I21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J21" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1294,7 +1299,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -1305,7 +1310,7 @@
         <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3">
@@ -1316,7 +1321,7 @@
         <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4">
@@ -1327,7 +1332,7 @@
         <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5">
@@ -1338,7 +1343,7 @@
         <v>155</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6">
@@ -1349,7 +1354,7 @@
         <v>156</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7">
@@ -1360,7 +1365,7 @@
         <v>157</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8">
@@ -1371,7 +1376,7 @@
         <v>158</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9">
@@ -1382,7 +1387,7 @@
         <v>159</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1404,7 +1409,7 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
@@ -1415,7 +1420,7 @@
         <v>160</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3">
@@ -1426,7 +1431,7 @@
         <v>161</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
@@ -1437,7 +1442,7 @@
         <v>162</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
@@ -1448,7 +1453,7 @@
         <v>163</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6">
@@ -1459,7 +1464,7 @@
         <v>164</v>
       </c>
       <c r="C6" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
@@ -1470,7 +1475,7 @@
         <v>165</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
@@ -1481,7 +1486,7 @@
         <v>166</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9">
@@ -1492,7 +1497,7 @@
         <v>167</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
@@ -1503,7 +1508,7 @@
         <v>168</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11">
@@ -1514,7 +1519,7 @@
         <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12">
@@ -1525,7 +1530,7 @@
         <v>170</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13">
@@ -1536,7 +1541,7 @@
         <v>171</v>
       </c>
       <c r="C13" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14">
@@ -1547,7 +1552,7 @@
         <v>172</v>
       </c>
       <c r="C14" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15">
@@ -1558,7 +1563,7 @@
         <v>173</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16">
@@ -1569,7 +1574,7 @@
         <v>174</v>
       </c>
       <c r="C16" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17">
@@ -1580,7 +1585,7 @@
         <v>175</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18">
@@ -1591,7 +1596,7 @@
         <v>176</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>